<commit_message>
Update for Wed Apr 11 18:59:03 2018
</commit_message>
<xml_diff>
--- a/distros/E/Excel-Writer-XLSX/t/regression/xlsx_files/chart_chartarea05.xlsx
+++ b/distros/E/Excel-Writer-XLSX/t/regression/xlsx_files/chart_chartarea05.xlsx
@@ -105,6 +105,14 @@
         </c:ser>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -135,7 +143,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>

</xml_diff>